<commit_message>
Added Diode, Began Routing
</commit_message>
<xml_diff>
--- a/Schematics/Rocket Control Board/Parts Explanation.xlsx
+++ b/Schematics/Rocket Control Board/Parts Explanation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RRS-Secret\Schematics\Rocket Control Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feldh\Desktop\Repositories\RRS-RCOS\Schematics\Rocket Control Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Rough Cortex Poinout" sheetId="1" r:id="rId1"/>
     <sheet name="Comprehensive Parts List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="160">
   <si>
     <t>Arduino Zero Core</t>
   </si>
@@ -506,11 +506,23 @@
   <si>
     <t>GLFR1608T2R2M-LR</t>
   </si>
+  <si>
+    <t>Regulator Diode</t>
+  </si>
+  <si>
+    <t>CTS05S40L3FCT-ND</t>
+  </si>
+  <si>
+    <t>SOD-882</t>
+  </si>
+  <si>
+    <t>Diode between USB and VIN-(Unregulated)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,13 +555,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,6 +656,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -679,6 +708,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -837,657 +883,654 @@
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="168.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2" hidden="1"/>
+    <col min="1" max="1" width="3.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="168.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
         <v>18</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="D21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
         <v>19</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
         <v>21</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
         <v>23</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="1">
         <v>24</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
         <v>25</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>11</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
         <v>26</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>13</v>
       </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
         <v>27</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>10</v>
       </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
         <v>28</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>12</v>
       </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
         <v>30</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
         <v>31</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
         <v>32</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
         <v>33</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="1">
         <v>34</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="1">
         <v>35</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="1">
         <v>36</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="1">
         <v>37</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="1">
         <v>38</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="1">
         <v>39</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="1">
         <v>40</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="1">
         <v>41</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="1">
         <v>42</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="1">
         <v>43</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" s="1">
         <v>44</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="1">
         <v>45</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="1">
         <v>46</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="1">
         <v>47</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="1">
         <v>48</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" s="1" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="G40:G41"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
@@ -1495,8 +1538,11 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1505,25 +1551,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.3984375" customWidth="1"/>
+    <col min="2" max="2" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
         <v>123</v>
       </c>
@@ -1531,13 +1577,13 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G2">
         <f>SUM(G4:G50)</f>
-        <v>12.59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12.94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -1563,7 +1609,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1590,7 +1636,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -1610,11 +1656,11 @@
         <v>109</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G18" si="0">D5*E5</f>
+        <f t="shared" ref="G5:G19" si="0">D5*E5</f>
         <v>0.43</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -1638,8 +1684,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B7" t="s">
@@ -1654,7 +1700,7 @@
       <c r="E7">
         <v>6</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G7">
@@ -1662,7 +1708,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -1686,8 +1732,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B9" t="s">
@@ -1702,7 +1748,7 @@
       <c r="E9">
         <v>2</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>146</v>
       </c>
       <c r="G9">
@@ -1710,7 +1756,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -1734,7 +1780,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -1758,7 +1804,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -1782,7 +1828,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -1806,7 +1852,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>135</v>
       </c>
@@ -1833,7 +1879,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -1857,7 +1903,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -1881,7 +1927,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -1905,7 +1951,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>147</v>
       </c>
@@ -1927,6 +1973,30 @@
       <c r="G18">
         <f t="shared" si="0"/>
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19">
+        <v>0.35</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>